<commit_message>
Change collumn names in photometricParam.xlsx
</commit_message>
<xml_diff>
--- a/tables/PhotometricParam.xlsx
+++ b/tables/PhotometricParam.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D28B99-E0F2-4E7B-8FC1-48986D3BB61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F6F08A-F600-4954-950A-8065D9B8965A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,54 +25,6 @@
     <t>ST</t>
   </si>
   <si>
-    <t>$M_{U}$</t>
-  </si>
-  <si>
-    <t>$M_{B}$</t>
-  </si>
-  <si>
-    <t>$M_{V}$</t>
-  </si>
-  <si>
-    <t>$M_{J}$</t>
-  </si>
-  <si>
-    <t>$M_{H}$</t>
-  </si>
-  <si>
-    <t>$M_{K}$</t>
-  </si>
-  <si>
-    <t>$(U-B)_{\rm 0}$</t>
-  </si>
-  <si>
-    <t>$(B-V)_{\rm 0}$</t>
-  </si>
-  <si>
-    <t>$(J-H)_{0}$</t>
-  </si>
-  <si>
-    <t>$(H-K)_{0}$</t>
-  </si>
-  <si>
-    <t>$BC_{U}$</t>
-  </si>
-  <si>
-    <t>$BC_{B}$</t>
-  </si>
-  <si>
-    <t>$BC_{V}$</t>
-  </si>
-  <si>
-    <t>$BC_{J}$</t>
-  </si>
-  <si>
-    <t>$BC_{H}$</t>
-  </si>
-  <si>
-    <t>$BC_{K}$</t>
-  </si>
-  <si>
     <t>O3V</t>
   </si>
   <si>
@@ -179,6 +131,54 @@
   </si>
   <si>
     <t>O9.5I</t>
+  </si>
+  <si>
+    <t>Mu</t>
+  </si>
+  <si>
+    <t>Mb</t>
+  </si>
+  <si>
+    <t>Mv</t>
+  </si>
+  <si>
+    <t>Mj</t>
+  </si>
+  <si>
+    <t>Mh</t>
+  </si>
+  <si>
+    <t>Mk</t>
+  </si>
+  <si>
+    <t>(U-B)0</t>
+  </si>
+  <si>
+    <t>(B-V)0</t>
+  </si>
+  <si>
+    <t>(J_H)0</t>
+  </si>
+  <si>
+    <t>(H-K)0</t>
+  </si>
+  <si>
+    <t>Bcu</t>
+  </si>
+  <si>
+    <t>BCb</t>
+  </si>
+  <si>
+    <t>BCv</t>
+  </si>
+  <si>
+    <t>BCj</t>
+  </si>
+  <si>
+    <t>BCh</t>
+  </si>
+  <si>
+    <t>BCk</t>
   </si>
 </sst>
 </file>
@@ -558,67 +558,73 @@
   <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
       </c>
       <c r="B2">
         <v>-7.31</v>
@@ -669,9 +675,9 @@
         <v>-4.87</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>-7.01</v>
@@ -722,9 +728,9 @@
         <v>-4.7300000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>-6.69</v>
@@ -775,9 +781,9 @@
         <v>-4.58</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>-6.56</v>
@@ -828,9 +834,9 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>-6.4</v>
@@ -881,9 +887,9 @@
         <v>-4.42</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>-6.24</v>
@@ -934,9 +940,9 @@
         <v>-4.34</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>-6.09</v>
@@ -987,9 +993,9 @@
         <v>-4.26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>-5.94</v>
@@ -1040,9 +1046,9 @@
         <v>-4.17</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>-5.79</v>
@@ -1093,9 +1099,9 @@
         <v>-4.08</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>-5.62</v>
@@ -1146,9 +1152,9 @@
         <v>-3.99</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>-5.48</v>
@@ -1199,9 +1205,9 @@
         <v>-3.9</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>-5.34</v>
@@ -1252,9 +1258,9 @@
         <v>-3.8</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>-7.63</v>
@@ -1305,9 +1311,9 @@
         <v>-4.8499999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>-7.49</v>
@@ -1358,9 +1364,9 @@
         <v>-4.7</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>-7.33</v>
@@ -1411,9 +1417,9 @@
         <v>-4.54</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>-7.25</v>
@@ -1464,9 +1470,9 @@
         <v>-4.46</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>-7.17</v>
@@ -1517,9 +1523,9 @@
         <v>-4.37</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>-7.07</v>
@@ -1570,9 +1576,9 @@
         <v>-4.28</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>-7</v>
@@ -1623,9 +1629,9 @@
         <v>-4.1900000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>-6.93</v>
@@ -1676,9 +1682,9 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>-6.84</v>
@@ -1729,9 +1735,9 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>-6.75</v>
@@ -1782,9 +1788,9 @@
         <v>-3.9</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>-6.66</v>
@@ -1835,9 +1841,9 @@
         <v>-3.8</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>-6.6</v>
@@ -1888,9 +1894,9 @@
         <v>-3.69</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>-7.85</v>
@@ -1941,9 +1947,9 @@
         <v>-4.6900000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>-7.82</v>
@@ -1994,9 +2000,9 @@
         <v>-4.55</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>-7.79</v>
@@ -2047,9 +2053,9 @@
         <v>-4.4000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>-7.78</v>
@@ -2100,9 +2106,9 @@
         <v>-4.33</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>-7.77</v>
@@ -2153,9 +2159,9 @@
         <v>-4.25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>-7.76</v>
@@ -2206,9 +2212,9 @@
         <v>-4.17</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>-7.76</v>
@@ -2259,9 +2265,9 @@
         <v>-4.09</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>-7.75</v>
@@ -2312,9 +2318,9 @@
         <v>-4.01</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>-7.73</v>
@@ -2365,9 +2371,9 @@
         <v>-3.93</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>-7.73</v>
@@ -2418,9 +2424,9 @@
         <v>-3.84</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>-7.7</v>
@@ -2471,9 +2477,9 @@
         <v>-3.75</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>-7.68</v>
@@ -2527,7 +2533,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Q1 A37 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32 A33 A34 A35 A36" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 A37 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32 A33 A34 A35 A36" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added guesses for spectral types B0 and B1 to PhotometricParams.xlsx
</commit_message>
<xml_diff>
--- a/tables/PhotometricParam.xlsx
+++ b/tables/PhotometricParam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F6F08A-F600-4954-950A-8065D9B8965A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639D4077-B870-4125-8428-2FA4501D26B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>ST</t>
   </si>
@@ -163,9 +163,6 @@
     <t>(H-K)0</t>
   </si>
   <si>
-    <t>Bcu</t>
-  </si>
-  <si>
     <t>BCb</t>
   </si>
   <si>
@@ -179,6 +176,27 @@
   </si>
   <si>
     <t>BCk</t>
+  </si>
+  <si>
+    <t>B0I</t>
+  </si>
+  <si>
+    <t>B1I</t>
+  </si>
+  <si>
+    <t>B0III</t>
+  </si>
+  <si>
+    <t>B1III</t>
+  </si>
+  <si>
+    <t>B0V</t>
+  </si>
+  <si>
+    <t>B1V</t>
+  </si>
+  <si>
+    <t>BCu</t>
   </si>
 </sst>
 </file>
@@ -555,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -604,22 +622,22 @@
         <v>46</v>
       </c>
       <c r="L1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>48</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>50</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>51</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -2528,6 +2546,90 @@
       </c>
       <c r="Q37">
         <v>-3.66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38">
+        <v>-6.33</v>
+      </c>
+      <c r="I38">
+        <v>-0.26</v>
+      </c>
+      <c r="N38">
+        <v>-2.76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39">
+        <v>-6.32</v>
+      </c>
+      <c r="I39">
+        <v>-0.26</v>
+      </c>
+      <c r="N39">
+        <v>-2.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40">
+        <v>-5.16</v>
+      </c>
+      <c r="I40">
+        <v>-0.26</v>
+      </c>
+      <c r="N40">
+        <v>-2.77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41">
+        <v>-5.01</v>
+      </c>
+      <c r="I41">
+        <v>-0.26</v>
+      </c>
+      <c r="N41">
+        <v>-2.58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42">
+        <v>-3.83</v>
+      </c>
+      <c r="I42">
+        <v>-0.26</v>
+      </c>
+      <c r="N42">
+        <v>-2.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43">
+        <v>-3.54</v>
+      </c>
+      <c r="I43">
+        <v>-0.26</v>
+      </c>
+      <c r="N43">
+        <v>-2.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added guesses for the logL/Lsun collumn in StellarParam.xlsx. Added a comparison for Ltrue and L based on the martin(2005a) models.
</commit_message>
<xml_diff>
--- a/tables/PhotometricParam.xlsx
+++ b/tables/PhotometricParam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639D4077-B870-4125-8428-2FA4501D26B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACD1499-2AA6-48F3-9C68-1EDBDDCE3F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed the guesses for the B spectral types from the tables
</commit_message>
<xml_diff>
--- a/tables/PhotometricParam.xlsx
+++ b/tables/PhotometricParam.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACD1499-2AA6-48F3-9C68-1EDBDDCE3F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F098406-16FD-480E-B01B-C1172239473B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>ST</t>
   </si>
@@ -176,24 +176,6 @@
   </si>
   <si>
     <t>BCk</t>
-  </si>
-  <si>
-    <t>B0I</t>
-  </si>
-  <si>
-    <t>B1I</t>
-  </si>
-  <si>
-    <t>B0III</t>
-  </si>
-  <si>
-    <t>B1III</t>
-  </si>
-  <si>
-    <t>B0V</t>
-  </si>
-  <si>
-    <t>B1V</t>
   </si>
   <si>
     <t>BCu</t>
@@ -573,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -622,7 +604,7 @@
         <v>46</v>
       </c>
       <c r="L1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="M1" t="s">
         <v>47</v>
@@ -2546,90 +2528,6 @@
       </c>
       <c r="Q37">
         <v>-3.66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38">
-        <v>-6.33</v>
-      </c>
-      <c r="I38">
-        <v>-0.26</v>
-      </c>
-      <c r="N38">
-        <v>-2.76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39">
-        <v>-6.32</v>
-      </c>
-      <c r="I39">
-        <v>-0.26</v>
-      </c>
-      <c r="N39">
-        <v>-2.6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40">
-        <v>-5.16</v>
-      </c>
-      <c r="I40">
-        <v>-0.26</v>
-      </c>
-      <c r="N40">
-        <v>-2.77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41">
-        <v>-5.01</v>
-      </c>
-      <c r="I41">
-        <v>-0.26</v>
-      </c>
-      <c r="N41">
-        <v>-2.58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42">
-        <v>-3.83</v>
-      </c>
-      <c r="I42">
-        <v>-0.26</v>
-      </c>
-      <c r="N42">
-        <v>-2.9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43">
-        <v>-3.54</v>
-      </c>
-      <c r="I43">
-        <v>-0.26</v>
-      </c>
-      <c r="N43">
-        <v>-2.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added objects, but their L is calculated with the JHK filters. So that part of the code is a bit modified. Also merged the dataframes for R,L, and M along the way.
</commit_message>
<xml_diff>
--- a/tables/PhotometricParam.xlsx
+++ b/tables/PhotometricParam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F098406-16FD-480E-B01B-C1172239473B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4A7A61-2A9E-4C00-97E6-1C120042A3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,9 +157,6 @@
     <t>(B-V)0</t>
   </si>
   <si>
-    <t>(J_H)0</t>
-  </si>
-  <si>
     <t>(H-K)0</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>BCu</t>
+  </si>
+  <si>
+    <t>(J-H)0</t>
   </si>
 </sst>
 </file>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -598,28 +598,28 @@
         <v>44</v>
       </c>
       <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
         <v>45</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
         <v>46</v>
       </c>
-      <c r="L1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>47</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>48</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>49</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>50</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>